<commit_message>
Finishing the previous TODO list
Fixed the project description
Fixed the 2v5 graphs
Chapter 2: References
Chapter 4:
         Bézier curve
         Classnames in sections
         Sequence of operations
         Images of start and end screen
         Image references
         Refactored UML
Chapter 5:
         AI interface
         AI appellation
         AI flowcharts references
         AI feature table
Chapter 6:
         Conclusion of the graphs
         Graph references
         AI ranking table
Chapter 7: Import the appendices
</commit_message>
<xml_diff>
--- a/docs/simulations.xlsx
+++ b/docs/simulations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>AI1</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t>AI5</t>
+  </si>
+  <si>
+    <t>AI1(K)</t>
+  </si>
+  <si>
+    <t>AI2(K)</t>
+  </si>
+  <si>
+    <t>AI3(K)</t>
+  </si>
+  <si>
+    <t>AI4(K)</t>
+  </si>
+  <si>
+    <t>AI5(K)</t>
   </si>
 </sst>
 </file>
@@ -358,15 +373,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -383,7 +398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -402,8 +417,15 @@
       <c r="F2">
         <v>551</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <f>SUM(C2:F2)/4</f>
+        <v>2184</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -422,8 +444,15 @@
       <c r="F3">
         <v>1688</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <f>SUM(B3,D3:F3)/4</f>
+        <v>6119.75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -442,8 +471,15 @@
       <c r="F4">
         <v>855</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <f>SUM(B4:C4,E4:F4)/4</f>
+        <v>3545.75</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -462,8 +498,15 @@
       <c r="F5">
         <v>1242</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <f>SUM(B5:D5,F5)/4</f>
+        <v>5533.75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -482,8 +525,137 @@
       <c r="F6">
         <v>5262</v>
       </c>
+      <c r="H6">
+        <f>SUM(B6:E6)/4</f>
+        <v>9267.5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <f>10000-SUM(B3:B6)/4</f>
+        <v>1627.25</v>
+      </c>
+      <c r="C8">
+        <f>10000-SUM(C2,C4:C6)/4</f>
+        <v>5311.25</v>
+      </c>
+      <c r="D8">
+        <f>10000-SUM(D2:D3,D5:D6)/4</f>
+        <v>2816.25</v>
+      </c>
+      <c r="E8">
+        <f>10000-SUM(E2:E4,E6)/4</f>
+        <v>4678.5</v>
+      </c>
+      <c r="F8">
+        <f>10000-SUM(F2:F5)/4</f>
+        <v>8916</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>9267.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>8916</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>6119.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>5533.75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>5311.25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>4678.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>3545.75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2816.25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>2184</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1627.25</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="B13:C22">
+    <sortCondition descending="1" ref="C13:C22"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>